<commit_message>
Update sample Excel file with tested column additions
- Excel file now includes tested CONDITION and ACTION columns
- Demonstrates proper column positioning and template values
- Validates end-to-end Add Column functionality

Co-Authored-By: sai.n@worldlink-us.com <sai.n@worldlink-us.com>
</commit_message>
<xml_diff>
--- a/rules/SampleRules.xlsx
+++ b/rules/SampleRules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>ACTION 1</t>
   </si>
@@ -41,6 +41,33 @@
   </si>
   <si>
     <t>customer.setBonus($param);</t>
+  </si>
+  <si>
+    <t>New Credit Check</t>
+  </si>
+  <si>
+    <t>customer.getCreditScore() &gt;= $param</t>
+  </si>
+  <si>
+    <t>CONDITION 2</t>
+  </si>
+  <si>
+    <t>customer.getStatus() == "$param"</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>SENIOR</t>
+  </si>
+  <si>
+    <t>PREMIUM</t>
+  </si>
+  <si>
+    <t>Loyalty Reward</t>
+  </si>
+  <si>
+    <t>customer.setLoyaltyPoints($param);</t>
   </si>
 </sst>
 </file>
@@ -444,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,39 +485,37 @@
           <t>NAME</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr" s="0">
-        <is>
-          <t>CONDITION 1</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr" s="0">
-        <is>
-          <t>CONDITION 2</t>
-        </is>
+      <c r="B1" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>9</v>
       </c>
       <c r="D1" t="s" s="0">
         <v>0</v>
       </c>
       <c r="E1" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr" s="0"/>
-      <c r="B2" t="inlineStr" s="0">
-        <is>
-          <t>customer.getAge() &gt;= $param</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr" s="0">
-        <is>
-          <t>customer.getStatus() == "$param"</t>
-        </is>
+      <c r="B2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>10</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>2</v>
       </c>
       <c r="E2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -500,20 +525,15 @@
           <t>Rule1</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr" s="0">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr" s="0">
-        <is>
-          <t>ACTIVE</t>
-        </is>
-      </c>
+      <c r="B3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0"/>
       <c r="D3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="E3" s="0"/>
+      <c r="F3"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr" s="0">
@@ -521,20 +541,15 @@
           <t>Rule2</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr" s="0">
-        <is>
-          <t>65</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr" s="0">
-        <is>
-          <t>SENIOR</t>
-        </is>
-      </c>
+      <c r="B4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0"/>
       <c r="D4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="E4" s="0"/>
+      <c r="F4"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr" s="0">
@@ -542,20 +557,15 @@
           <t>Rule3</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr" s="0">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr" s="0">
-        <is>
-          <t>PREMIUM</t>
-        </is>
-      </c>
+      <c r="B5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0"/>
       <c r="D5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="E5" s="0"/>
+      <c r="F5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add Drools integration with proper decision table format
- Add drools-rules-spring-boot-starter:10.1.0 dependency to pom.xml
- Create DroolsService for rule processing, validation, and column naming
- Update ExcelService to use Drools-compliant column naming (CONDITION/ACTION vs numbered)
- Add proper Drools template syntax support (customer.getAge() >= $param)
- Update frontend components for Drools column management
- Add rule execution endpoint with Drools validation
- Create Drools-compliant sample Excel file with RuleSet/RuleTable structure
- Implement smart column positioning following Drools conventions
- Add column deletion validation ensuring minimum CONDITION/ACTION requirements

Tested: Column addition/deletion works with proper Drools naming and positioning
Co-Authored-By: sai.n@worldlink-us.com <sai.n@worldlink-us.com>
</commit_message>
<xml_diff>
--- a/rules/SampleRules.xlsx
+++ b/rules/SampleRules.xlsx
@@ -14,60 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
-  <si>
-    <t>ACTION 1</t>
-  </si>
-  <si>
-    <t>New Age Verification</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>CONDITION3</t>
   </si>
   <si>
     <t>customer.setDiscount($param);</t>
   </si>
   <si>
-    <t>customer.getAge() &gt; $param</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.2</t>
+    <t>customer.isVip() == $param</t>
+  </si>
+  <si>
+    <t>0.05</t>
   </si>
   <si>
     <t>0.15</t>
   </si>
   <si>
-    <t>Bonus Action</t>
-  </si>
-  <si>
-    <t>customer.setBonus($param);</t>
-  </si>
-  <si>
-    <t>New Credit Check</t>
-  </si>
-  <si>
-    <t>customer.getCreditScore() &gt;= $param</t>
-  </si>
-  <si>
-    <t>CONDITION 2</t>
-  </si>
-  <si>
-    <t>customer.getStatus() == "$param"</t>
-  </si>
-  <si>
-    <t>ACTIVE</t>
-  </si>
-  <si>
-    <t>SENIOR</t>
-  </si>
-  <si>
-    <t>PREMIUM</t>
-  </si>
-  <si>
-    <t>Loyalty Reward</t>
-  </si>
-  <si>
-    <t>customer.setLoyaltyPoints($param);</t>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>ACTION2</t>
+  </si>
+  <si>
+    <t>customer.setStatus("$param");</t>
   </si>
 </sst>
 </file>
@@ -471,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,90 +455,186 @@
     <row r="1">
       <c r="A1" t="inlineStr" s="0">
         <is>
-          <t>NAME</t>
-        </is>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
+          <t>RuleSet</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr" s="0">
+        <is>
+          <t>CustomerRules</t>
+        </is>
+      </c>
+      <c r="D1" s="0"/>
+      <c r="F1" s="0"/>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr" s="0"/>
-      <c r="B2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" t="inlineStr" s="0">
+        <is>
+          <t>Import</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr" s="0">
+        <is>
+          <t>com.example.model.Customer</t>
+        </is>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="F2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr" s="0">
         <is>
-          <t>Rule1</t>
-        </is>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C3" s="0"/>
-      <c r="D3" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="E3" s="0"/>
-      <c r="F3"/>
+          <t>Variables</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr" s="0">
+        <is>
+          <t>Customer customer</t>
+        </is>
+      </c>
+      <c r="D3" s="0"/>
+      <c r="F3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr" s="0">
         <is>
-          <t>Rule2</t>
-        </is>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0"/>
-      <c r="D4" t="s" s="0">
+          <t>Sequential</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr" s="0">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="D4" s="0"/>
+      <c r="F4" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr" s="0">
+        <is>
+          <t>RuleTable</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr" s="0">
+        <is>
+          <t>CustomerDiscountRules</t>
+        </is>
+      </c>
+      <c r="D6" s="0"/>
+      <c r="F6" s="0"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr" s="0">
+        <is>
+          <t>NAME</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr" s="0">
+        <is>
+          <t>CONDITION</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr" s="0">
+        <is>
+          <t>CONDITION2</t>
+        </is>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr" s="0"/>
+      <c r="B8" t="inlineStr" s="0">
+        <is>
+          <t>customer.getAge() &gt;= $param</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr" s="0">
+        <is>
+          <t>customer.getStatus() == "$param"</t>
+        </is>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr" s="0">
+        <is>
+          <t>YoungAdultRule</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr" s="0">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr" s="0">
+        <is>
+          <t>ACTIVE</t>
+        </is>
+      </c>
+      <c r="D9" s="0"/>
+      <c r="E9" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F9" s="0"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr" s="0">
+        <is>
+          <t>SeniorRule</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr" s="0">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr" s="0">
+        <is>
+          <t>SENIOR</t>
+        </is>
+      </c>
+      <c r="D10" s="0"/>
+      <c r="E10" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="E4" s="0"/>
-      <c r="F4"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr" s="0">
-        <is>
-          <t>Rule3</t>
-        </is>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="C5" s="0"/>
-      <c r="D5" t="s" s="0">
+      <c r="F10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr" s="0">
+        <is>
+          <t>PremiumRule</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr" s="0">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr" s="0">
+        <is>
+          <t>PREMIUM</t>
+        </is>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="E5" s="0"/>
-      <c r="F5"/>
+      <c r="F11" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implement dynamic horizontal scrolling for Drools decision tables
- Updated CSS to use overflow-x: auto for dynamic scroll bar behavior
- Scroll bar only appears when table content exceeds container width
- When few columns fit naturally, no scroll bar is shown
- Table layout changed to auto for dynamic column sizing
- Maintained static column widths (150px-250px) and text wrapping
- Events column remains sticky on the right during scrolling
- Template value validation and column naming without numbers preserved
- Tested with 8 columns - content fits naturally without scroll bar

Co-Authored-By: sai.n@worldlink-us.com <sai.n@worldlink-us.com>
</commit_message>
<xml_diff>
--- a/rules/SampleRules.xlsx
+++ b/rules/SampleRules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>ACTION</t>
   </si>
@@ -41,6 +41,45 @@
   </si>
   <si>
     <t>customer.setStatus("$param");</t>
+  </si>
+  <si>
+    <t>YoungAdultRule</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>44sds</t>
+  </si>
+  <si>
+    <t>SeniorRule</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>SENIOR</t>
+  </si>
+  <si>
+    <t>PremiumRule</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>PREMIUM</t>
+  </si>
+  <si>
+    <t>CONDITION</t>
+  </si>
+  <si>
+    <t>customer.getBalance() &gt;= 1000</t>
+  </si>
+  <si>
+    <t>customer.getCreditScore() &gt;= 700</t>
   </si>
 </sst>
 </file>
@@ -444,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,7 +503,10 @@
         </is>
       </c>
       <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
       <c r="F1" s="0"/>
+      <c r="G1"/>
+      <c r="H1"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr" s="0">
@@ -478,7 +520,10 @@
         </is>
       </c>
       <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
       <c r="F2" s="0"/>
+      <c r="G2"/>
+      <c r="H2"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr" s="0">
@@ -492,7 +537,10 @@
         </is>
       </c>
       <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
       <c r="F3" s="0"/>
+      <c r="G3"/>
+      <c r="H3"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr" s="0">
@@ -506,7 +554,10 @@
         </is>
       </c>
       <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
       <c r="F4" s="0"/>
+      <c r="G4"/>
+      <c r="H4"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr" s="0">
@@ -520,7 +571,10 @@
         </is>
       </c>
       <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
       <c r="F6" s="0"/>
+      <c r="G6"/>
+      <c r="H6"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr" s="0">
@@ -542,9 +596,15 @@
         <v>1</v>
       </c>
       <c r="E7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
         <v>0</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="H7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -564,77 +624,71 @@
         <v>3</v>
       </c>
       <c r="E8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s" s="0">
+      <c r="H8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr" s="0">
-        <is>
-          <t>YoungAdultRule</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr" s="0">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr" s="0">
-        <is>
-          <t>ACTIVE</t>
-        </is>
+      <c r="A9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>11</v>
       </c>
       <c r="D9" s="0"/>
-      <c r="E9" t="s" s="0">
-        <v>4</v>
-      </c>
+      <c r="E9" s="0"/>
       <c r="F9" s="0"/>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr" s="0">
-        <is>
-          <t>SeniorRule</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr" s="0">
-        <is>
-          <t>65</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr" s="0">
-        <is>
-          <t>SENIOR</t>
-        </is>
+      <c r="A10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>15</v>
       </c>
       <c r="D10" s="0"/>
-      <c r="E10" t="s" s="0">
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="0"/>
+      <c r="H10"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr" s="0">
-        <is>
-          <t>PremiumRule</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr" s="0">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr" s="0">
-        <is>
-          <t>PREMIUM</t>
-        </is>
+      <c r="A11" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>18</v>
       </c>
       <c r="D11" s="0"/>
-      <c r="E11" t="s" s="0">
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="0"/>
+      <c r="H11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update SampleRules.xlsx with test data for dynamic scrolling verification
Co-Authored-By: sai.n@worldlink-us.com <sai.n@worldlink-us.com>
</commit_message>
<xml_diff>
--- a/rules/SampleRules.xlsx
+++ b/rules/SampleRules.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="23">
   <si>
     <t>ACTION</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>customer.getCreditScore() &gt;= 700</t>
+  </si>
+  <si>
+    <t>customer.getAge() &gt;= $param</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,8 +508,7 @@
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
-      <c r="G1"/>
-      <c r="H1"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr" s="0">
@@ -522,8 +524,7 @@
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
-      <c r="G2"/>
-      <c r="H2"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr" s="0">
@@ -539,8 +540,7 @@
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
-      <c r="G3"/>
-      <c r="H3"/>
+      <c r="G3" s="0"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr" s="0">
@@ -556,8 +556,7 @@
       <c r="D4" s="0"/>
       <c r="E4" s="0"/>
       <c r="F4" s="0"/>
-      <c r="G4"/>
-      <c r="H4"/>
+      <c r="G4" s="0"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr" s="0">
@@ -573,8 +572,7 @@
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
-      <c r="G6"/>
-      <c r="H6"/>
+      <c r="G6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr" s="0">
@@ -599,12 +597,9 @@
         <v>19</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="G7" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s" s="0">
         <v>7</v>
       </c>
     </row>
@@ -627,12 +622,9 @@
         <v>20</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
         <v>2</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s" s="0">
         <v>8</v>
       </c>
     </row>
@@ -648,11 +640,10 @@
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" t="s">
+      <c r="F9" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="H9"/>
+      <c r="G9" s="0"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
@@ -666,11 +657,10 @@
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" t="s">
+      <c r="F10" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H10"/>
+      <c r="G10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
@@ -684,11 +674,10 @@
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" t="s">
+      <c r="F11" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H11"/>
+      <c r="G11" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>